<commit_message>
Corrections to errors in tables!
</commit_message>
<xml_diff>
--- a/Tabele/Wyniki Eksperymentu.xlsx
+++ b/Tabele/Wyniki Eksperymentu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esmira\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E1BA679-E273-4F91-AC70-A4964772EE7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D770009E-E70E-43E4-BC0A-CE0F2FE35EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="750" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -198,7 +198,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -206,7 +206,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -218,11 +218,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -230,9 +228,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -241,6 +236,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -587,7 +585,7 @@
   <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -608,29 +606,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13" t="s">
+      <c r="H1" s="15"/>
+      <c r="I1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="15" t="s">
+      <c r="J1" s="15"/>
+      <c r="K1" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -641,28 +639,28 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -673,33 +671,33 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="8">
         <v>104.54</v>
       </c>
-      <c r="D3" s="10">
-        <v>0</v>
-      </c>
-      <c r="E3" s="10">
-        <v>91.16</v>
-      </c>
-      <c r="F3" s="10">
+      <c r="D3" s="8">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8">
+        <v>98.16</v>
+      </c>
+      <c r="F3" s="8">
+        <v>2</v>
+      </c>
+      <c r="G3" s="8">
+        <v>84.75</v>
+      </c>
+      <c r="H3" s="8">
         <v>1</v>
       </c>
-      <c r="G3" s="10">
-        <v>84.75</v>
-      </c>
-      <c r="H3" s="10">
-        <v>1</v>
-      </c>
-      <c r="I3" s="10">
+      <c r="I3" s="8">
         <v>78.52</v>
       </c>
-      <c r="J3" s="10">
-        <v>0</v>
-      </c>
-      <c r="K3" s="10">
+      <c r="J3" s="8">
+        <v>0</v>
+      </c>
+      <c r="K3" s="8">
         <f>SUM(I3,G3,E3,C3)</f>
-        <v>358.96999999999997</v>
+        <v>365.96999999999997</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -714,33 +712,33 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="8">
         <v>96.85</v>
       </c>
-      <c r="D4" s="10">
-        <v>0</v>
-      </c>
-      <c r="E4" s="10">
-        <v>89.23</v>
-      </c>
-      <c r="F4" s="10">
-        <v>0</v>
-      </c>
-      <c r="G4" s="10">
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8">
+        <v>93.23</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8">
         <v>118.09</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="8">
         <v>4</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="8">
         <v>106.98</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="8">
         <v>1</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="8">
         <f t="shared" ref="K4:K9" si="0">SUM(I4,G4,E4,C4)</f>
-        <v>411.15</v>
+        <v>415.15</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -756,31 +754,31 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="8">
         <v>110.98</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="8">
         <v>1</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="8">
         <v>123.02</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="8">
         <v>3</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="8">
         <v>99.11</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="8">
         <v>2</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="8">
         <v>69.75</v>
       </c>
-      <c r="J5" s="10">
-        <v>0</v>
-      </c>
-      <c r="K5" s="10">
+      <c r="J5" s="8">
+        <v>0</v>
+      </c>
+      <c r="K5" s="8">
         <f t="shared" si="0"/>
         <v>402.86</v>
       </c>
@@ -793,31 +791,31 @@
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="8">
         <v>78.31</v>
       </c>
-      <c r="D6" s="10">
-        <v>0</v>
-      </c>
-      <c r="E6" s="10">
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8">
         <v>78.319999999999993</v>
       </c>
-      <c r="F6" s="10">
-        <v>0</v>
-      </c>
-      <c r="G6" s="10">
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
         <v>27.98</v>
       </c>
-      <c r="H6" s="10">
-        <v>0</v>
-      </c>
-      <c r="I6" s="10">
+      <c r="H6" s="8">
+        <v>0</v>
+      </c>
+      <c r="I6" s="8">
         <v>55.43</v>
       </c>
-      <c r="J6" s="10">
-        <v>0</v>
-      </c>
-      <c r="K6" s="10">
+      <c r="J6" s="8">
+        <v>0</v>
+      </c>
+      <c r="K6" s="8">
         <f t="shared" si="0"/>
         <v>240.04</v>
       </c>
@@ -830,31 +828,31 @@
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="8">
         <v>73.73</v>
       </c>
-      <c r="D7" s="10">
-        <v>0</v>
-      </c>
-      <c r="E7" s="10">
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
         <v>65.25</v>
       </c>
-      <c r="F7" s="10">
-        <v>0</v>
-      </c>
-      <c r="G7" s="10">
+      <c r="F7" s="8">
+        <v>0</v>
+      </c>
+      <c r="G7" s="8">
         <v>37.770000000000003</v>
       </c>
-      <c r="H7" s="10">
-        <v>0</v>
-      </c>
-      <c r="I7" s="10">
+      <c r="H7" s="8">
+        <v>0</v>
+      </c>
+      <c r="I7" s="8">
         <v>59.01</v>
       </c>
-      <c r="J7" s="10">
-        <v>0</v>
-      </c>
-      <c r="K7" s="10">
+      <c r="J7" s="8">
+        <v>0</v>
+      </c>
+      <c r="K7" s="8">
         <f t="shared" si="0"/>
         <v>235.76</v>
       </c>
@@ -864,40 +862,40 @@
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="13">
         <f>AVERAGE(C3:C5)</f>
         <v>104.12333333333333</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="13">
         <f t="shared" ref="E8:I8" si="1">AVERAGE(E3:E5)</f>
-        <v>101.13666666666666</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="16">
+        <v>104.80333333333333</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="13">
         <f t="shared" si="1"/>
         <v>100.64999999999999</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="13">
         <f t="shared" si="1"/>
         <v>85.083333333333329</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="16">
+      <c r="K8" s="13">
         <f t="shared" si="0"/>
-        <v>390.99333333333334</v>
+        <v>394.65999999999997</v>
       </c>
       <c r="Q8" s="1"/>
     </row>
@@ -905,38 +903,38 @@
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="13">
         <f>AVERAGE(C6:C7)</f>
         <v>76.02000000000001</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="13">
         <f t="shared" ref="E9:I9" si="2">AVERAGE(E6:E7)</f>
         <v>71.784999999999997</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="13">
         <f t="shared" si="2"/>
         <v>32.875</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="13">
         <f t="shared" si="2"/>
         <v>57.22</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="K9" s="16">
+      <c r="K9" s="13">
         <f t="shared" si="0"/>
         <v>237.9</v>
       </c>
@@ -962,29 +960,29 @@
       <c r="Q14" s="1"/>
     </row>
     <row r="15" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="12" t="s">
+      <c r="A15" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13" t="s">
+      <c r="D15" s="15"/>
+      <c r="E15" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13" t="s">
+      <c r="F15" s="15"/>
+      <c r="G15" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13" t="s">
+      <c r="H15" s="15"/>
+      <c r="I15" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="15" t="s">
+      <c r="J15" s="15"/>
+      <c r="K15" s="12" t="s">
         <v>22</v>
       </c>
       <c r="L15" s="1"/>
@@ -1001,422 +999,302 @@
       <c r="B16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="I16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="J16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K16" s="10" t="s">
+      <c r="K16" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="8">
         <v>148.26</v>
       </c>
-      <c r="D17" s="10">
-        <v>2</v>
-      </c>
-      <c r="E17" s="10">
+      <c r="D17" s="8">
+        <v>1</v>
+      </c>
+      <c r="E17" s="8">
         <v>88.99</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="8">
         <v>1</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G17" s="8">
         <v>74.55</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H17" s="8">
         <v>1</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="8">
         <v>139.97</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="8">
         <v>1</v>
       </c>
-      <c r="K17" s="10">
-        <f>SUM(I17,G17,E17,C17)</f>
+      <c r="K17" s="8">
+        <f t="shared" ref="K17:K23" si="3">SUM(I17,G17,E17,C17)</f>
         <v>451.77</v>
       </c>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="8">
         <v>124.65</v>
       </c>
-      <c r="D18" s="10">
-        <v>0</v>
-      </c>
-      <c r="E18" s="10">
+      <c r="D18" s="8">
+        <v>0</v>
+      </c>
+      <c r="E18" s="8">
         <v>79.95</v>
       </c>
-      <c r="F18" s="10">
-        <v>0</v>
-      </c>
-      <c r="G18" s="10">
+      <c r="F18" s="8">
+        <v>1</v>
+      </c>
+      <c r="G18" s="8">
         <v>67.91</v>
       </c>
-      <c r="H18" s="10">
-        <v>0</v>
-      </c>
-      <c r="I18" s="10">
+      <c r="H18" s="8">
+        <v>0</v>
+      </c>
+      <c r="I18" s="8">
         <v>220.28</v>
       </c>
-      <c r="J18" s="10">
-        <v>5</v>
-      </c>
-      <c r="K18" s="10">
-        <f>SUM(I18,G18,E18,C18)</f>
+      <c r="J18" s="8">
+        <v>3</v>
+      </c>
+      <c r="K18" s="8">
+        <f t="shared" si="3"/>
         <v>492.78999999999996</v>
       </c>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="8">
         <v>131.93</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="8">
         <v>1</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="8">
         <v>82.91</v>
       </c>
-      <c r="F19" s="10">
-        <v>0</v>
-      </c>
-      <c r="G19" s="10">
+      <c r="F19" s="8">
+        <v>1</v>
+      </c>
+      <c r="G19" s="8">
         <v>68.37</v>
       </c>
-      <c r="H19" s="10">
-        <v>0</v>
-      </c>
-      <c r="I19" s="10">
+      <c r="H19" s="8">
+        <v>0</v>
+      </c>
+      <c r="I19" s="8">
         <v>90.91</v>
       </c>
-      <c r="J19" s="10">
-        <v>0</v>
-      </c>
-      <c r="K19" s="10">
-        <f>SUM(I19,G19,E19,C19)</f>
+      <c r="J19" s="8">
+        <v>0</v>
+      </c>
+      <c r="K19" s="8">
+        <f t="shared" si="3"/>
         <v>374.12</v>
       </c>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="8">
         <v>87.17</v>
       </c>
-      <c r="D20" s="10">
-        <v>0</v>
-      </c>
-      <c r="E20" s="10">
+      <c r="D20" s="8">
+        <v>0</v>
+      </c>
+      <c r="E20" s="8">
         <v>52.02</v>
       </c>
-      <c r="F20" s="10">
-        <v>0</v>
-      </c>
-      <c r="G20" s="10">
+      <c r="F20" s="8">
+        <v>0</v>
+      </c>
+      <c r="G20" s="8">
         <v>20.93</v>
       </c>
-      <c r="H20" s="10">
-        <v>0</v>
-      </c>
-      <c r="I20" s="10">
+      <c r="H20" s="8">
+        <v>0</v>
+      </c>
+      <c r="I20" s="8">
         <v>54.21</v>
       </c>
-      <c r="J20" s="10">
-        <v>0</v>
-      </c>
-      <c r="K20" s="10">
-        <f>SUM(I20,G20,E20,C20)</f>
+      <c r="J20" s="8">
+        <v>0</v>
+      </c>
+      <c r="K20" s="8">
+        <f t="shared" si="3"/>
         <v>214.32999999999998</v>
       </c>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="8">
         <v>82.58</v>
       </c>
-      <c r="D21" s="10">
-        <v>0</v>
-      </c>
-      <c r="E21" s="10">
+      <c r="D21" s="8">
+        <v>0</v>
+      </c>
+      <c r="E21" s="8">
         <v>51.25</v>
       </c>
-      <c r="F21" s="10">
-        <v>0</v>
-      </c>
-      <c r="G21" s="10">
+      <c r="F21" s="8">
+        <v>0</v>
+      </c>
+      <c r="G21" s="8">
         <v>22.62</v>
       </c>
-      <c r="H21" s="10">
-        <v>0</v>
-      </c>
-      <c r="I21" s="10">
+      <c r="H21" s="8">
+        <v>0</v>
+      </c>
+      <c r="I21" s="8">
         <v>56.66</v>
       </c>
-      <c r="J21" s="10">
-        <v>0</v>
-      </c>
-      <c r="K21" s="10">
-        <f>SUM(I21,G21,E21,C21)</f>
+      <c r="J21" s="8">
+        <v>0</v>
+      </c>
+      <c r="K21" s="8">
+        <f t="shared" si="3"/>
         <v>213.11</v>
       </c>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="9">
         <f>AVERAGE(C17:C19)</f>
         <v>134.94666666666666</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="11">
-        <f t="shared" ref="E22:I22" si="3">AVERAGE(E17:E19)</f>
+      <c r="E22" s="9">
+        <f t="shared" ref="E22:I22" si="4">AVERAGE(E17:E19)</f>
         <v>83.95</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F22" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="9">
+        <f t="shared" si="4"/>
+        <v>70.276666666666657</v>
+      </c>
+      <c r="H22" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G22" s="11">
+      <c r="I22" s="9">
+        <f t="shared" si="4"/>
+        <v>150.38666666666666</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="9">
         <f t="shared" si="3"/>
-        <v>70.276666666666657</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I22" s="11">
-        <f t="shared" si="3"/>
-        <v>150.38666666666666</v>
-      </c>
-      <c r="J22" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K22" s="11">
-        <f>SUM(I22,G22,E22,C22)</f>
         <v>439.55999999999995</v>
       </c>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="9">
         <f>AVERAGE(C20:C21)</f>
         <v>84.875</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="11">
-        <f t="shared" ref="E23:I23" si="4">AVERAGE(E20:E21)</f>
+      <c r="E23" s="9">
+        <f t="shared" ref="E23:I23" si="5">AVERAGE(E20:E21)</f>
         <v>51.635000000000005</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="F23" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="11">
-        <f t="shared" si="4"/>
+      <c r="G23" s="9">
+        <f t="shared" si="5"/>
         <v>21.774999999999999</v>
       </c>
-      <c r="H23" s="17" t="s">
+      <c r="H23" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I23" s="11">
-        <f t="shared" si="4"/>
+      <c r="I23" s="9">
+        <f t="shared" si="5"/>
         <v>55.435000000000002</v>
       </c>
-      <c r="J23" s="17" t="s">
+      <c r="J23" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="K23" s="11">
-        <f>SUM(I23,G23,E23,C23)</f>
+      <c r="K23" s="9">
+        <f t="shared" si="3"/>
         <v>213.72000000000003</v>
       </c>
       <c r="L23" s="4"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L32" s="5"/>
     </row>
     <row r="33" spans="12:12" x14ac:dyDescent="0.25">
@@ -1433,12 +1311,6 @@
     </row>
     <row r="37" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L37" s="7"/>
-    </row>
-    <row r="38" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L38" s="8"/>
-    </row>
-    <row r="39" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L39" s="8"/>
     </row>
     <row r="40" spans="12:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="L40" s="2"/>

</xml_diff>